<commit_message>
data: Change files containing substance names and IDs
In the XLSX and RDS files containing substance names and IDs, one name
has changed and one substance has been added.
</commit_message>
<xml_diff>
--- a/data-raw/create_USIS_data/subst_usData_brute.xlsx
+++ b/data-raw/create_USIS_data/subst_usData_brute.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="2356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="2358">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -851,7 +851,7 @@
     <t xml:space="preserve">0472</t>
   </si>
   <si>
-    <t xml:space="preserve">Butyl Cellosolve Acetate 0473 tert-Butyl Chromate (as CrO3), prior to 5/30/2006</t>
+    <t xml:space="preserve">Butyl Cellosolve Acetate</t>
   </si>
   <si>
     <t xml:space="preserve">0477</t>
@@ -7080,12 +7080,18 @@
   </si>
   <si>
     <t xml:space="preserve">Ziram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tert-Butyl Chromate (as CrO3), prior to 5/30/2006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -7404,10 +7410,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -20837,6 +20843,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1245">
+      <c r="A1245" t="s">
+        <v>2356</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>2357</v>
+      </c>
+      <c r="C1245" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>